<commit_message>
fixed daily procents calculation
</commit_message>
<xml_diff>
--- a/Keeper/ByFunctional/DepositProcessing/DepositsCalculationScheme.xlsx
+++ b/Keeper/ByFunctional/DepositProcessing/DepositsCalculationScheme.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="77">
   <si>
     <t>показать отчет по депозиту</t>
   </si>
@@ -222,12 +222,6 @@
     <t>decimal Balance</t>
   </si>
   <si>
-    <t>decimal DayProfit</t>
-  </si>
-  <si>
-    <t>decimal NotPaidProfit</t>
-  </si>
-  <si>
     <t>decimal DayDevaluation</t>
   </si>
   <si>
@@ -299,6 +293,15 @@
   </si>
   <si>
     <t xml:space="preserve">         Account BankAccount</t>
+  </si>
+  <si>
+    <t>decimal DepoRate</t>
+  </si>
+  <si>
+    <t>decimal DayProcents</t>
+  </si>
+  <si>
+    <t>decimal NotPaidProcents</t>
   </si>
 </sst>
 </file>
@@ -348,9 +351,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -361,6 +361,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -716,7 +719,7 @@
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -727,25 +730,25 @@
       <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="2"/>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="2"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -754,7 +757,7 @@
       <c r="E10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="2"/>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -763,7 +766,7 @@
       <c r="E11" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="2"/>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -772,7 +775,7 @@
       <c r="E12" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="2"/>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -815,7 +818,7 @@
       <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="6" t="s">
         <v>34</v>
       </c>
     </row>
@@ -823,43 +826,43 @@
       <c r="B20" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F22" s="2"/>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F23" s="2"/>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>35</v>
       </c>
-      <c r="F24" s="2"/>
+      <c r="F24" s="6"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F25" s="2"/>
+      <c r="F25" s="6"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>37</v>
       </c>
-      <c r="F26" s="2"/>
+      <c r="F26" s="6"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>38</v>
       </c>
-      <c r="F27" s="2"/>
+      <c r="F27" s="6"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C28" s="1" t="s">
@@ -946,10 +949,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B7:F44"/>
+  <dimension ref="B7:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,7 +964,7 @@
   <sheetData>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>51</v>
@@ -971,33 +974,33 @@
       </c>
     </row>
     <row r="8" spans="2:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="9" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="10" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="5" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="4" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1023,17 +1026,17 @@
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.25">
@@ -1058,96 +1061,101 @@
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>61</v>
+      <c r="D29" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
-        <v>62</v>
+      <c r="C30" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>43</v>
+      <c r="D36" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
devaluation in predictions and on aggregate deposits view
</commit_message>
<xml_diff>
--- a/Keeper/ByFunctional/DepositProcessing/DepositsCalculationScheme.xlsx
+++ b/Keeper/ByFunctional/DepositProcessing/DepositsCalculationScheme.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="83">
   <si>
     <t>показать отчет по депозиту</t>
   </si>
@@ -308,6 +308,18 @@
   </si>
   <si>
     <t>decimal CurrencyRate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          decimal TotalPercentInUsd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          decimal EstimatedDevaluationInUsd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          decimal EstimatedCurrencyRateOnFinish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          decimal CurrentDevaluationInUsd</t>
   </si>
 </sst>
 </file>
@@ -955,10 +967,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B7:F46"/>
+  <dimension ref="B7:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD29"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,122 +1064,142 @@
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
-        <v>40</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deposit related class into visio diagram
</commit_message>
<xml_diff>
--- a/Keeper/ByFunctional/DepositProcessing/DepositsCalculationScheme.xlsx
+++ b/Keeper/ByFunctional/DepositProcessing/DepositsCalculationScheme.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="89">
   <si>
     <t>показать отчет по депозиту</t>
   </si>
@@ -320,6 +320,24 @@
   </si>
   <si>
     <t xml:space="preserve">          decimal CurrentDevaluationInUsd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> public class DepositRateLine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        public DateTime DateFrom { get; set; }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        public decimal AmountFrom { get; set; }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        public decimal AmountTo { get; set; }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        public decimal Rate { get; set; }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        [NonSerialized] public int AccountId;</t>
   </si>
 </sst>
 </file>
@@ -353,7 +371,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -361,11 +379,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -383,12 +438,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF6D6D"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -398,6 +462,1041 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>409573</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3571877" cy="3238500"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7762873" y="5410200"/>
+          <a:ext cx="3571877" cy="3238500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent5">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>public class DepositCalculationData</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>       </a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>public DepositStates State { get; set; }</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        </a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>public List&lt;</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>DepositTransaction</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>&gt; Traffic { get; set; }</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        public List&lt;</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>DepositDailyLine</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>&gt; DailyTable { get; set; }</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        </a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>public decimal TotalMyIns { get; set; }</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>       </a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>public decimal TotalPercent { get; set; }</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>       </a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>public decimal TotalPercentInUsd { get; set; }</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        </a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>public decimal TotalMyOuts { get; set; }</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        </a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>public decimal TotalMyOutsInUsd { get; set; }</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        </a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>public decimal CurrentBalance </a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>{ get { return TotalMyIns + TotalPercent - TotalMyOuts; } }</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        </a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>public decimal CurrentProfitInUsd { get; set; }</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        </a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>public decimal CurrentDevaluationInUsd { get; set; }</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        public decimal EstimatedProcentsInThisMonth { get; set; }</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        </a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>public decimal EstimatedProcents { get; set; }</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>       </a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>public decimal EstimatedCurrencyRateOnFinish { get; set; }</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        </a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>public decimal EstimatedDevaluationInUsd { get; set; }</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        public decimal EstimatedProfitInUsd { get; set; }</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3914775" cy="1304925"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12953999" y="5067299"/>
+          <a:ext cx="3914775" cy="1304925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent5">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> public class DepositTransaction</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>       </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>public DateTime Timestamp { get; set; }</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        public DepositTransactionTypes TransactionType { get; set; }</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        public Decimal Amount { get; set; }</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        public CurrencyCodes Currency { get; set; }</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        public Decimal AmountInUsd { get; set; }</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        public string Comment { get; set; }</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12954000" y="7134226"/>
+          <a:ext cx="3971925" cy="1295399"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> public class </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" smtClean="0">
+              <a:solidFill>
+                <a:srgbClr val="FF6D6D"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>DepositTransaction</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    public DateTime Timestamp { get; set; }</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        public DepositTransactionTypes TransactionType { get; set; }</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        public Decimal Amount { get; set; }</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        public CurrencyCodes Currency { get; set; }</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        public Decimal AmountInUsd { get; set; }</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        public string Comment { get; set; }</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -967,20 +2066,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B7:F50"/>
+  <dimension ref="B7:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.7109375" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>66</v>
       </c>
@@ -991,7 +2091,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>67</v>
       </c>
@@ -1003,7 +2103,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>68</v>
       </c>
@@ -1015,196 +2115,191 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="K15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q15" s="1"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="F19" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="K19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="F20" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="K20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="F21" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="F22" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="F23" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D27" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D29" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
+      <c r="F24" s="8" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
+      <c r="Q24" s="10"/>
+    </row>
+    <row r="25" spans="3:17" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>59</v>
+      </c>
+      <c r="F25" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>79</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>46</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>77</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D35" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
+        <v>82</v>
+      </c>
+      <c r="F32" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
+    <row r="33" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>48</v>
+      </c>
+      <c r="F33" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
+    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
deposit devaluation evaluating is improved
</commit_message>
<xml_diff>
--- a/Keeper/ByFunctional/DepositProcessing/DepositsCalculationScheme.xlsx
+++ b/Keeper/ByFunctional/DepositProcessing/DepositsCalculationScheme.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="97">
   <si>
     <t>показать отчет по депозиту</t>
   </si>
@@ -313,12 +313,6 @@
     <t xml:space="preserve">          decimal TotalPercentInUsd</t>
   </si>
   <si>
-    <t xml:space="preserve">          decimal EstimatedDevaluationInUsd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          decimal EstimatedCurrencyRateOnFinish</t>
-  </si>
-  <si>
     <t xml:space="preserve">          decimal CurrentDevaluationInUsd</t>
   </si>
   <si>
@@ -338,6 +332,61 @@
   </si>
   <si>
     <t xml:space="preserve">        [NonSerialized] public int AccountId;</t>
+  </si>
+  <si>
+    <t>DepositDailyLine</t>
+  </si>
+  <si>
+    <t>DepositTransaction</t>
+  </si>
+  <si>
+    <t>DepositEstimations</t>
+  </si>
+  <si>
+    <t>CurrencyRateOnThisMonthPayment</t>
+  </si>
+  <si>
+    <t>ProcentsInThisMonth</t>
+  </si>
+  <si>
+    <t>CurrencyRateOnFinish</t>
+  </si>
+  <si>
+    <t>DevaluationInUsd</t>
+  </si>
+  <si>
+    <t>ProfitInUsd</t>
+  </si>
+  <si>
+    <t>ProcentsUpToFinish</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DepositEstimations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Estimations</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -435,13 +484,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1836,7 +1885,7 @@
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="10" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1847,25 +1896,25 @@
       <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="6"/>
+      <c r="G6" s="10"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="6"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="6"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="6"/>
+      <c r="G9" s="10"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -1874,7 +1923,7 @@
       <c r="E10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="6"/>
+      <c r="G10" s="10"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -1883,7 +1932,7 @@
       <c r="E11" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="6"/>
+      <c r="G11" s="10"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -1892,7 +1941,7 @@
       <c r="E12" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="6"/>
+      <c r="G12" s="10"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -1935,7 +1984,7 @@
       <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="10" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1943,43 +1992,43 @@
       <c r="B20" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="6"/>
+      <c r="F20" s="10"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="6"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F22" s="6"/>
+      <c r="F22" s="10"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F23" s="6"/>
+      <c r="F23" s="10"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>35</v>
       </c>
-      <c r="F24" s="6"/>
+      <c r="F24" s="10"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F25" s="6"/>
+      <c r="F25" s="10"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>37</v>
       </c>
-      <c r="F26" s="6"/>
+      <c r="F26" s="10"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>38</v>
       </c>
-      <c r="F27" s="6"/>
+      <c r="F27" s="10"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C28" s="1" t="s">
@@ -2066,10 +2115,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B7:Q37"/>
+  <dimension ref="B7:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2127,7 +2176,7 @@
         <v>35</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q15" s="1"/>
     </row>
@@ -2136,23 +2185,29 @@
         <v>36</v>
       </c>
       <c r="K16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>37</v>
       </c>
+      <c r="F17" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="K17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>38</v>
       </c>
+      <c r="F18" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="K18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="3:17" x14ac:dyDescent="0.25">
@@ -2160,36 +2215,36 @@
         <v>71</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="K19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="7" t="s">
         <v>57</v>
       </c>
       <c r="K20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>73</v>
       </c>
-      <c r="F21" s="8" t="s">
-        <v>74</v>
+      <c r="F21" s="7" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="7" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2197,25 +2252,22 @@
       <c r="C23" t="s">
         <v>40</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>55</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q24" s="10"/>
-    </row>
-    <row r="25" spans="3:17" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="Q24" s="9"/>
+    </row>
+    <row r="25" spans="3:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>59</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="26" spans="3:17" x14ac:dyDescent="0.25">
@@ -2227,12 +2279,15 @@
       <c r="C27" t="s">
         <v>44</v>
       </c>
+      <c r="F27" s="1" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="28" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>79</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="6" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2240,7 +2295,7 @@
       <c r="C29" t="s">
         <v>45</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F29" s="7" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2248,7 +2303,7 @@
       <c r="C30" t="s">
         <v>46</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="7" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2256,44 +2311,59 @@
       <c r="C31" t="s">
         <v>77</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F31" s="7" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="32" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>82</v>
-      </c>
-      <c r="F32" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F32" s="7" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="33" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
-        <v>48</v>
-      </c>
-      <c r="F33" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="F33" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>81</v>
+    <row r="35" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F35" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>80</v>
+      <c r="F36" s="6" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>50</v>
+      <c r="F37" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F40" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F41" s="8" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deposits view shows forecast
</commit_message>
<xml_diff>
--- a/Keeper/ByFunctional/DepositProcessing/DepositsCalculationScheme.xlsx
+++ b/Keeper/ByFunctional/DepositProcessing/DepositsCalculationScheme.xlsx
@@ -343,24 +343,6 @@
     <t>DepositEstimations</t>
   </si>
   <si>
-    <t>CurrencyRateOnThisMonthPayment</t>
-  </si>
-  <si>
-    <t>ProcentsInThisMonth</t>
-  </si>
-  <si>
-    <t>CurrencyRateOnFinish</t>
-  </si>
-  <si>
-    <t>DevaluationInUsd</t>
-  </si>
-  <si>
-    <t>ProfitInUsd</t>
-  </si>
-  <si>
-    <t>ProcentsUpToFinish</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">          </t>
     </r>
@@ -387,6 +369,24 @@
       </rPr>
       <t xml:space="preserve"> Estimations</t>
     </r>
+  </si>
+  <si>
+    <t>Period PeriodForThisMonthPayment</t>
+  </si>
+  <si>
+    <t>Period PeriodForUpToEndPayment</t>
+  </si>
+  <si>
+    <t>decimal ProcentsInThisMonth</t>
+  </si>
+  <si>
+    <t>decimal ProcentsUpToFinish</t>
+  </si>
+  <si>
+    <t>decimal DevaluationInUsd</t>
+  </si>
+  <si>
+    <t>decimal ProfitInUsd</t>
   </si>
 </sst>
 </file>
@@ -515,702 +515,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>409573</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="3571877" cy="3238500"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7762873" y="5410200"/>
-          <a:ext cx="3571877" cy="3238500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent5">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>public class DepositCalculationData</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>       </a:t>
-          </a:r>
-          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>public DepositStates State { get; set; }</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>        </a:t>
-          </a:r>
-          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>public List&lt;</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>DepositTransaction</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>&gt; Traffic { get; set; }</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>        public List&lt;</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>DepositDailyLine</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>&gt; DailyTable { get; set; }</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>        </a:t>
-          </a:r>
-          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>public decimal TotalMyIns { get; set; }</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>       </a:t>
-          </a:r>
-          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>public decimal TotalPercent { get; set; }</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>       </a:t>
-          </a:r>
-          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>public decimal TotalPercentInUsd { get; set; }</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>        </a:t>
-          </a:r>
-          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>public decimal TotalMyOuts { get; set; }</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>        </a:t>
-          </a:r>
-          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>public decimal TotalMyOutsInUsd { get; set; }</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>        </a:t>
-          </a:r>
-          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>public decimal CurrentBalance </a:t>
-          </a:r>
-          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>{ get { return TotalMyIns + TotalPercent - TotalMyOuts; } }</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>        </a:t>
-          </a:r>
-          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>public decimal CurrentProfitInUsd { get; set; }</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>        </a:t>
-          </a:r>
-          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>public decimal CurrentDevaluationInUsd { get; set; }</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>        public decimal EstimatedProcentsInThisMonth { get; set; }</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>        </a:t>
-          </a:r>
-          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>public decimal EstimatedProcents { get; set; }</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>       </a:t>
-          </a:r>
-          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>public decimal EstimatedCurrencyRateOnFinish { get; set; }</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>        </a:t>
-          </a:r>
-          <a:endParaRPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>public decimal EstimatedDevaluationInUsd { get; set; }</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>        public decimal EstimatedProfitInUsd { get; set; }</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:endParaRPr lang="ru-RU" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
@@ -2118,14 +1422,14 @@
   <dimension ref="B7:Q41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.7109375" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
     <col min="17" max="17" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2175,7 +1479,7 @@
       <c r="C15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>81</v>
       </c>
       <c r="Q15" s="1"/>
@@ -2184,7 +1488,7 @@
       <c r="C16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K16" t="s">
+      <c r="H16" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2195,7 +1499,7 @@
       <c r="F17" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K17" t="s">
+      <c r="H17" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2206,7 +1510,7 @@
       <c r="F18" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="K18" t="s">
+      <c r="H18" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2217,7 +1521,7 @@
       <c r="F19" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="K19" t="s">
+      <c r="H19" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2228,7 +1532,7 @@
       <c r="F20" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="K20" t="s">
+      <c r="H20" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2325,7 +1629,7 @@
     </row>
     <row r="33" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>65</v>
@@ -2343,27 +1647,27 @@
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F37" s="7" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F38" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F39" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F40" s="7" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F41" s="8" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>